<commit_message>
readme a jour avec l'explicatif des routes
</commit_message>
<xml_diff>
--- a/Conception/LBS-stories-LP1.xlsx
+++ b/Conception/LBS-stories-LP1.xlsx
@@ -14,6 +14,8 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">Feuille1!$A$1:$G$47</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">Feuille1!$A$1:$G$47</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0" vbProcedure="false">Feuille1!$A$1:$G$47</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0" vbProcedure="false">Feuille1!$A$1:$G$47</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0" vbProcedure="false">Feuille1!$A$1:$G$47</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -25,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="100">
   <si>
     <t xml:space="preserve">USER STORIES pour l'application LE BON SANDWICH</t>
   </si>
@@ -114,10 +116,7 @@
     <t xml:space="preserve">sandwich par catégorie</t>
   </si>
   <si>
-    <t xml:space="preserve">obtenir la liste des sandwichs d'une catégorie</t>
-  </si>
-  <si>
-    <t xml:space="preserve">categories/id/sandwichs</t>
+    <t xml:space="preserve">Obtenir la liste des sandwichs d'une catégorie</t>
   </si>
   <si>
     <t xml:space="preserve">\controllerCategorie\getSandwichs()</t>
@@ -129,7 +128,7 @@
     <t xml:space="preserve">Obtenir la liste des sandwich avec filtrage sur le type de pain et l'image</t>
   </si>
   <si>
-    <t xml:space="preserve">sandwichs/type&amp;image ?</t>
+    <t xml:space="preserve">sandwichs?type=&amp;img=</t>
   </si>
   <si>
     <t xml:space="preserve">\controllerSandwich\getListFilter()</t>
@@ -141,7 +140,7 @@
     <t xml:space="preserve">Obtenir la liste des sandwichs avec pagination</t>
   </si>
   <si>
-    <t xml:space="preserve">sandwichs ?</t>
+    <t xml:space="preserve">sandwichs?page=&amp;size=</t>
   </si>
   <si>
     <t xml:space="preserve">\controllerSandwich\getListPaging()</t>
@@ -153,16 +152,13 @@
     <t xml:space="preserve">Obtenir la description détaillée d'un sandwich avec les tailles, prix et catégories du sandwich sous forme de liste imbriquée</t>
   </si>
   <si>
-    <t xml:space="preserve">sandwichs/id ?</t>
-  </si>
-  <si>
     <t xml:space="preserve">\controllerSandwich\getSandwich()</t>
   </si>
   <si>
     <t xml:space="preserve">créer une commande</t>
   </si>
   <si>
-    <t xml:space="preserve">créer une nouvelle commande  (vide) :  la date de livraison (date-heure) et les coordonnées du client sont transmises – retourne 1 token d'identification de la commande</t>
+    <t xml:space="preserve">Créer une nouvelle commande  (vide) :  la date de livraison (date-heure) et les coordonnées du client sont transmises – retourne 1 token d'identification de la commande</t>
   </si>
   <si>
     <t xml:space="preserve">POST</t>
@@ -174,7 +170,7 @@
     <t xml:space="preserve">ajouter  sandwich</t>
   </si>
   <si>
-    <t xml:space="preserve">ajouter un sandwich à une commande existante – en accord avec l'état de la commande – transmet les id de sandwich et taille et la quantité</t>
+    <t xml:space="preserve">Ajouter un sandwich à une commande existante – en accord avec l'état de la commande – transmet les id de sandwich et taille et la quantité</t>
   </si>
   <si>
     <t xml:space="preserve">\controllerSandwich\create()</t>
@@ -183,7 +179,7 @@
     <t xml:space="preserve">Modifier une commande</t>
   </si>
   <si>
-    <t xml:space="preserve">modifier une commande existante : date de livraison</t>
+    <t xml:space="preserve">Modifier une commande existante : date de livraison</t>
   </si>
   <si>
     <t xml:space="preserve">PUT</t>
@@ -195,7 +191,7 @@
     <t xml:space="preserve">Payer une commande</t>
   </si>
   <si>
-    <t xml:space="preserve">payer une commande en transmettant des coordonnées bancaires – (n°carte+date-expiration)</t>
+    <t xml:space="preserve">Payer une commande en transmettant des coordonnées bancaires – (n°carte+date-expiration)</t>
   </si>
   <si>
     <t xml:space="preserve">\controllerCommande\buy()</t>
@@ -204,7 +200,7 @@
     <t xml:space="preserve">état de la commande</t>
   </si>
   <si>
-    <t xml:space="preserve">obtenir la commande pour suivre son état</t>
+    <t xml:space="preserve">Obtenir la commande pour suivre son état</t>
   </si>
   <si>
     <t xml:space="preserve">\controllerCommande\state()</t>
@@ -213,7 +209,7 @@
     <t xml:space="preserve">supprimer sandwich</t>
   </si>
   <si>
-    <t xml:space="preserve">supprimer un sandwich dans une commande</t>
+    <t xml:space="preserve">Supprimer un sandwich dans une commande</t>
   </si>
   <si>
     <t xml:space="preserve">DELETE</t>
@@ -225,7 +221,7 @@
     <t xml:space="preserve">modifier un item d'une commande (sandwich, taille, quantité)</t>
   </si>
   <si>
-    <t xml:space="preserve">modifier 1 élément d'une commande, en accord avec l'état de la commande.</t>
+    <t xml:space="preserve">Modifier 1 élément d'une commande, en accord avec l'état de la commande.</t>
   </si>
   <si>
     <t xml:space="preserve">\controllerCommande\change()</t>
@@ -246,19 +242,19 @@
     <t xml:space="preserve">liste des commandes</t>
   </si>
   <si>
-    <t xml:space="preserve">liste des commandes, filtrées sur l'état , triée par date de livraison et ordre de création – permet au point de vente de planifier la préparation des commandes</t>
+    <t xml:space="preserve">Liste des commandes, filtrées sur l'état , triée par date de livraison et ordre de création – permet au point de vente de planifier la préparation des commandes</t>
   </si>
   <si>
     <t xml:space="preserve">détail d'une commande</t>
   </si>
   <si>
-    <t xml:space="preserve">accès au détail complet d'une commande, avec la liste des items, les noms des sandwichs et leur taille sous la forme de ressources imbriqués</t>
+    <t xml:space="preserve">Accès au détail complet d'une commande, avec la liste des items, les noms des sandwichs et leur taille sous la forme de ressources imbriqués</t>
   </si>
   <si>
     <t xml:space="preserve">changement d'état d'une commande</t>
   </si>
   <si>
-    <t xml:space="preserve">changement de l'état d'une commande – vérification de la validité de la transition</t>
+    <t xml:space="preserve">Changement de l'état d'une commande – vérification de la validité de la transition</t>
   </si>
   <si>
     <t xml:space="preserve">STORIES CONCERNANT LA GESTION DE LA CARTE DE FIDELITE</t>
@@ -267,7 +263,7 @@
     <t xml:space="preserve">s'authentifier pour utiliser sa carte</t>
   </si>
   <si>
-    <t xml:space="preserve">authentification  http basic, retourne un token jwt</t>
+    <t xml:space="preserve">Authentification  http basic, retourne un token jwt</t>
   </si>
   <si>
     <t xml:space="preserve">accéder à sa carte de fidélité : montant + réduction</t>
@@ -279,13 +275,13 @@
     <t xml:space="preserve">paiement fidélisé</t>
   </si>
   <si>
-    <t xml:space="preserve">payer une commande en utilisant la carte : le montant est crédité sur la carte, on peut utiliser la réduction issue de la carte de fidélité – le montant cumulé est remis à 0 – le token jwt est nécessaire</t>
+    <t xml:space="preserve">Payer une commande en utilisant la carte : le montant est crédité sur la carte, on peut utiliser la réduction issue de la carte de fidélité – le montant cumulé est remis à 0 – le token jwt est nécessaire</t>
   </si>
   <si>
     <t xml:space="preserve">créer sa carte de fidélité</t>
   </si>
   <si>
-    <t xml:space="preserve">créer une carte de fidélité – retourne un identifiant de carte </t>
+    <t xml:space="preserve">Créer une carte de fidélité – retourne un identifiant de carte </t>
   </si>
   <si>
     <t xml:space="preserve">STORIES CONCERNANT LE BACKEND DE GESTION</t>
@@ -294,25 +290,25 @@
     <t xml:space="preserve">lister les sandwichs</t>
   </si>
   <si>
-    <t xml:space="preserve">lister les sandwichs  disponibles par catégories</t>
+    <t xml:space="preserve">Lister les sandwichs  disponibles par catégories</t>
   </si>
   <si>
     <t xml:space="preserve">supprimer un sandwich</t>
   </si>
   <si>
-    <t xml:space="preserve">supprimer 1 sandwich dans la liste</t>
+    <t xml:space="preserve">Supprimer 1 sandwich dans la liste</t>
   </si>
   <si>
     <t xml:space="preserve">ajouter un sandwich</t>
   </si>
   <si>
-    <t xml:space="preserve">ajouter un sandwich dans la liste, en indiquant sa catégorie – gérer le token csrf – gérer les tailles et prix</t>
+    <t xml:space="preserve">Ajouter un sandwich dans la liste, en indiquant sa catégorie – gérer le token csrf – gérer les tailles et prix</t>
   </si>
   <si>
     <t xml:space="preserve">modifier 1 sandwich</t>
   </si>
   <si>
-    <t xml:space="preserve">modifier la description, le nom ou le prix pour chaque taille d'un sandwich</t>
+    <t xml:space="preserve">Modifier la description, le nom ou le prix pour chaque taille d'un sandwich</t>
   </si>
   <si>
     <t xml:space="preserve">s'authentifier comme staff gestionnaire</t>
@@ -340,7 +336,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="12">
+  <fonts count="11">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -389,11 +385,6 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <b val="true"/>
@@ -484,7 +475,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -525,11 +516,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -553,19 +540,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -649,23 +636,23 @@
   <dimension ref="A1:V65536"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J16" activeCellId="0" sqref="J16"/>
+      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="7.56122448979592"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.71938775510204"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="26.1887755102041"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="54.9438775510204"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.1479591836735"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="16.469387755102"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="25.3775510204082"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="36.7908163265306"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="9.71938775510204"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="24.4591836734694"/>
-    <col collapsed="false" hidden="false" max="22" min="11" style="0" width="9.71938775510204"/>
-    <col collapsed="false" hidden="false" max="1025" min="23" style="0" width="19.1683673469388"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="7.29081632653061"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.44897959183673"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="25.3775510204082"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="53.7244897959184"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.6071428571429"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="24.8367346938776"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="35.9081632653061"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="9.44897959183673"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="23.7602040816327"/>
+    <col collapsed="false" hidden="false" max="22" min="11" style="0" width="9.44897959183673"/>
+    <col collapsed="false" hidden="false" max="1025" min="23" style="0" width="18.6275510204082"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -860,7 +847,7 @@
         <v>15</v>
       </c>
       <c r="I7" s="7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J7" s="2"/>
       <c r="K7" s="2"/>
@@ -902,7 +889,7 @@
         <v>19</v>
       </c>
       <c r="I8" s="7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J8" s="2"/>
       <c r="K8" s="2"/>
@@ -944,7 +931,7 @@
         <v>23</v>
       </c>
       <c r="I9" s="7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J9" s="2"/>
       <c r="K9" s="2"/>
@@ -986,7 +973,7 @@
         <v>27</v>
       </c>
       <c r="I10" s="7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J10" s="2"/>
       <c r="K10" s="2"/>
@@ -1021,11 +1008,9 @@
       <c r="F11" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="G11" s="9" t="s">
+      <c r="G11" s="9"/>
+      <c r="H11" s="9" t="s">
         <v>30</v>
-      </c>
-      <c r="H11" s="9" t="s">
-        <v>31</v>
       </c>
       <c r="I11" s="7" t="n">
         <v>0</v>
@@ -1052,10 +1037,10 @@
         <v>1</v>
       </c>
       <c r="C12" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="D12" s="8" t="s">
         <v>32</v>
-      </c>
-      <c r="D12" s="8" t="s">
-        <v>33</v>
       </c>
       <c r="E12" s="7" t="n">
         <v>3</v>
@@ -1064,13 +1049,13 @@
         <v>13</v>
       </c>
       <c r="G12" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="H12" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="H12" s="9" t="s">
-        <v>35</v>
-      </c>
       <c r="I12" s="7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J12" s="2"/>
       <c r="K12" s="2"/>
@@ -1094,10 +1079,10 @@
         <v>1</v>
       </c>
       <c r="C13" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="D13" s="8" t="s">
         <v>36</v>
-      </c>
-      <c r="D13" s="8" t="s">
-        <v>37</v>
       </c>
       <c r="E13" s="7" t="n">
         <v>3</v>
@@ -1106,13 +1091,13 @@
         <v>13</v>
       </c>
       <c r="G13" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="H13" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="H13" s="9" t="s">
-        <v>39</v>
-      </c>
       <c r="I13" s="7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J13" s="2"/>
       <c r="K13" s="2"/>
@@ -1136,10 +1121,10 @@
         <v>1</v>
       </c>
       <c r="C14" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="D14" s="8" t="s">
         <v>40</v>
-      </c>
-      <c r="D14" s="8" t="s">
-        <v>41</v>
       </c>
       <c r="E14" s="7" t="n">
         <v>3</v>
@@ -1148,13 +1133,13 @@
         <v>13</v>
       </c>
       <c r="G14" s="9" t="s">
-        <v>42</v>
+        <v>26</v>
       </c>
       <c r="H14" s="9" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="I14" s="7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J14" s="2"/>
       <c r="K14" s="2"/>
@@ -1178,20 +1163,20 @@
         <v>1</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E15" s="7" t="n">
         <v>4</v>
       </c>
       <c r="F15" s="9" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G15" s="9"/>
       <c r="H15" s="9" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="I15" s="7" t="n">
         <v>0</v>
@@ -1218,20 +1203,20 @@
         <v>1</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E16" s="7" t="n">
         <v>6</v>
       </c>
       <c r="F16" s="9" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G16" s="9"/>
       <c r="H16" s="9" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="I16" s="7" t="n">
         <v>0</v>
@@ -1258,20 +1243,20 @@
         <v>1</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E17" s="7" t="n">
         <v>4</v>
       </c>
       <c r="F17" s="9" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="G17" s="9"/>
       <c r="H17" s="9" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="I17" s="7" t="n">
         <v>0</v>
@@ -1298,20 +1283,20 @@
         <v>1</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E18" s="7" t="n">
         <v>3</v>
       </c>
       <c r="F18" s="9" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G18" s="9"/>
       <c r="H18" s="9" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="I18" s="7" t="n">
         <v>0</v>
@@ -1338,10 +1323,10 @@
         <v>1</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E19" s="7" t="n">
         <v>2</v>
@@ -1350,8 +1335,8 @@
         <v>13</v>
       </c>
       <c r="G19" s="9"/>
-      <c r="H19" s="10" t="s">
-        <v>60</v>
+      <c r="H19" s="9" t="s">
+        <v>58</v>
       </c>
       <c r="I19" s="7" t="n">
         <v>0</v>
@@ -1378,20 +1363,20 @@
         <v>2</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E20" s="7" t="n">
         <v>3</v>
       </c>
       <c r="F20" s="9" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="G20" s="9"/>
       <c r="H20" s="9" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="I20" s="7" t="n">
         <v>0</v>
@@ -1418,20 +1403,20 @@
         <v>2</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E21" s="7" t="n">
         <v>3</v>
       </c>
       <c r="F21" s="9" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="G21" s="9"/>
       <c r="H21" s="9" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="I21" s="7" t="n">
         <v>0</v>
@@ -1458,10 +1443,10 @@
         <v>2</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E22" s="7" t="n">
         <v>4</v>
@@ -1471,7 +1456,7 @@
       </c>
       <c r="G22" s="9"/>
       <c r="H22" s="9" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="I22" s="7" t="n">
         <v>0</v>
@@ -1491,30 +1476,30 @@
       <c r="V22" s="2"/>
     </row>
     <row r="23" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A23" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="B23" s="11"/>
-      <c r="C23" s="11"/>
-      <c r="D23" s="11"/>
-      <c r="E23" s="11"/>
-      <c r="F23" s="11"/>
-      <c r="G23" s="11"/>
-      <c r="H23" s="11"/>
-      <c r="I23" s="11"/>
-      <c r="J23" s="12"/>
-      <c r="K23" s="12"/>
-      <c r="L23" s="12"/>
-      <c r="M23" s="12"/>
-      <c r="N23" s="12"/>
-      <c r="O23" s="12"/>
-      <c r="P23" s="12"/>
-      <c r="Q23" s="12"/>
-      <c r="R23" s="12"/>
-      <c r="S23" s="12"/>
-      <c r="T23" s="12"/>
-      <c r="U23" s="12"/>
-      <c r="V23" s="12"/>
+      <c r="A23" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="B23" s="10"/>
+      <c r="C23" s="10"/>
+      <c r="D23" s="10"/>
+      <c r="E23" s="10"/>
+      <c r="F23" s="10"/>
+      <c r="G23" s="10"/>
+      <c r="H23" s="10"/>
+      <c r="I23" s="10"/>
+      <c r="J23" s="11"/>
+      <c r="K23" s="11"/>
+      <c r="L23" s="11"/>
+      <c r="M23" s="11"/>
+      <c r="N23" s="11"/>
+      <c r="O23" s="11"/>
+      <c r="P23" s="11"/>
+      <c r="Q23" s="11"/>
+      <c r="R23" s="11"/>
+      <c r="S23" s="11"/>
+      <c r="T23" s="11"/>
+      <c r="U23" s="11"/>
+      <c r="V23" s="11"/>
     </row>
     <row r="24" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="6" t="s">
@@ -1566,10 +1551,10 @@
         <v>1</v>
       </c>
       <c r="C25" s="8" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E25" s="7" t="n">
         <v>3</v>
@@ -1604,10 +1589,10 @@
         <v>1</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E26" s="7" t="n">
         <v>3</v>
@@ -1642,16 +1627,16 @@
         <v>1</v>
       </c>
       <c r="C27" s="8" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E27" s="7" t="n">
         <v>3</v>
       </c>
       <c r="F27" s="9" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="G27" s="9"/>
       <c r="H27" s="9"/>
@@ -1674,7 +1659,7 @@
     </row>
     <row r="28" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
@@ -1684,19 +1669,19 @@
       <c r="G28" s="4"/>
       <c r="H28" s="4"/>
       <c r="I28" s="4"/>
-      <c r="J28" s="12"/>
-      <c r="K28" s="12"/>
-      <c r="L28" s="12"/>
-      <c r="M28" s="12"/>
-      <c r="N28" s="12"/>
-      <c r="O28" s="12"/>
-      <c r="P28" s="12"/>
-      <c r="Q28" s="12"/>
-      <c r="R28" s="12"/>
-      <c r="S28" s="12"/>
-      <c r="T28" s="12"/>
-      <c r="U28" s="12"/>
-      <c r="V28" s="12"/>
+      <c r="J28" s="11"/>
+      <c r="K28" s="11"/>
+      <c r="L28" s="11"/>
+      <c r="M28" s="11"/>
+      <c r="N28" s="11"/>
+      <c r="O28" s="11"/>
+      <c r="P28" s="11"/>
+      <c r="Q28" s="11"/>
+      <c r="R28" s="11"/>
+      <c r="S28" s="11"/>
+      <c r="T28" s="11"/>
+      <c r="U28" s="11"/>
+      <c r="V28" s="11"/>
     </row>
     <row r="29" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="6" t="s">
@@ -1741,23 +1726,23 @@
       <c r="V29" s="2"/>
     </row>
     <row r="30" customFormat="false" ht="36.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A30" s="13" t="n">
+      <c r="A30" s="12" t="n">
         <v>200</v>
       </c>
       <c r="B30" s="7" t="n">
         <v>1</v>
       </c>
-      <c r="C30" s="14" t="s">
-        <v>79</v>
-      </c>
-      <c r="D30" s="15" t="s">
-        <v>80</v>
+      <c r="C30" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="D30" s="14" t="s">
+        <v>78</v>
       </c>
       <c r="E30" s="7" t="n">
         <v>5</v>
       </c>
       <c r="F30" s="9" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G30" s="9"/>
       <c r="H30" s="9"/>
@@ -1786,10 +1771,10 @@
         <v>1</v>
       </c>
       <c r="C31" s="8" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D31" s="8" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E31" s="7" t="n">
         <v>5</v>
@@ -1824,16 +1809,16 @@
         <v>1</v>
       </c>
       <c r="C32" s="8" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D32" s="8" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E32" s="7" t="n">
         <v>6</v>
       </c>
       <c r="F32" s="9" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G32" s="9"/>
       <c r="H32" s="9"/>
@@ -1862,16 +1847,16 @@
         <v>3</v>
       </c>
       <c r="C33" s="8" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D33" s="8" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E33" s="7" t="n">
         <v>4</v>
       </c>
       <c r="F33" s="9" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G33" s="9"/>
       <c r="H33" s="9"/>
@@ -1894,7 +1879,7 @@
     </row>
     <row r="34" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="4" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B34" s="4"/>
       <c r="C34" s="4"/>
@@ -1904,19 +1889,19 @@
       <c r="G34" s="4"/>
       <c r="H34" s="4"/>
       <c r="I34" s="4"/>
-      <c r="J34" s="12"/>
-      <c r="K34" s="12"/>
-      <c r="L34" s="12"/>
-      <c r="M34" s="12"/>
-      <c r="N34" s="12"/>
-      <c r="O34" s="12"/>
-      <c r="P34" s="12"/>
-      <c r="Q34" s="12"/>
-      <c r="R34" s="12"/>
-      <c r="S34" s="12"/>
-      <c r="T34" s="12"/>
-      <c r="U34" s="12"/>
-      <c r="V34" s="12"/>
+      <c r="J34" s="11"/>
+      <c r="K34" s="11"/>
+      <c r="L34" s="11"/>
+      <c r="M34" s="11"/>
+      <c r="N34" s="11"/>
+      <c r="O34" s="11"/>
+      <c r="P34" s="11"/>
+      <c r="Q34" s="11"/>
+      <c r="R34" s="11"/>
+      <c r="S34" s="11"/>
+      <c r="T34" s="11"/>
+      <c r="U34" s="11"/>
+      <c r="V34" s="11"/>
     </row>
     <row r="35" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="6" t="s">
@@ -1968,10 +1953,10 @@
         <v>1</v>
       </c>
       <c r="C36" s="8" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D36" s="8" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E36" s="7" t="n">
         <v>3</v>
@@ -2006,16 +1991,16 @@
         <v>2</v>
       </c>
       <c r="C37" s="8" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D37" s="8" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E37" s="7" t="n">
         <v>4</v>
       </c>
       <c r="F37" s="9" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="G37" s="9"/>
       <c r="H37" s="9"/>
@@ -2044,16 +2029,16 @@
         <v>1</v>
       </c>
       <c r="C38" s="8" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D38" s="8" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E38" s="7" t="n">
         <v>4</v>
       </c>
       <c r="F38" s="9" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G38" s="9"/>
       <c r="H38" s="9"/>
@@ -2082,16 +2067,16 @@
         <v>2</v>
       </c>
       <c r="C39" s="8" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D39" s="8" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E39" s="7" t="n">
         <v>3</v>
       </c>
       <c r="F39" s="9" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="G39" s="9"/>
       <c r="H39" s="9"/>
@@ -2120,16 +2105,16 @@
         <v>1</v>
       </c>
       <c r="C40" s="8" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D40" s="8" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E40" s="7" t="n">
         <v>4</v>
       </c>
       <c r="F40" s="9" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G40" s="9"/>
       <c r="H40" s="9"/>
@@ -2158,10 +2143,10 @@
         <v>3</v>
       </c>
       <c r="C41" s="8" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D41" s="8" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="E41" s="7" t="n">
         <v>4</v>
@@ -2191,8 +2176,8 @@
     <row r="42" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="1"/>
       <c r="B42" s="1"/>
-      <c r="C42" s="16"/>
-      <c r="D42" s="16"/>
+      <c r="C42" s="15"/>
+      <c r="D42" s="15"/>
       <c r="E42" s="1"/>
       <c r="F42" s="2"/>
       <c r="G42" s="2"/>
@@ -2215,8 +2200,8 @@
     <row r="43" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="1"/>
       <c r="B43" s="1"/>
-      <c r="C43" s="16"/>
-      <c r="D43" s="16"/>
+      <c r="C43" s="15"/>
+      <c r="D43" s="15"/>
       <c r="F43" s="2"/>
       <c r="G43" s="2"/>
       <c r="H43" s="2"/>
@@ -2238,13 +2223,13 @@
     <row r="44" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="1"/>
       <c r="B44" s="1"/>
-      <c r="C44" s="16"/>
-      <c r="D44" s="17" t="s">
-        <v>100</v>
-      </c>
-      <c r="E44" s="18" t="n">
+      <c r="C44" s="15"/>
+      <c r="D44" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="E44" s="17" t="n">
         <f aca="false">I41*E41+I40*E40+I39*E39+I38*E38+I37*E37+I36*E36+I33*E33+I32*E32+I31*E31+I30*E30+I27*E27+I26*E26+I25*E25+I22*E22+I21*E21+I20*E20+I19*E19+I18*E18+I17*E17+I16*E16+I15*E15+I14*E14+I13*E13+I12*E12+I11*E11+I10*E10+I9*E9+I8*E8+I7*E7</f>
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="F44" s="2"/>
       <c r="G44" s="2"/>
@@ -2267,11 +2252,11 @@
     <row r="45" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="1"/>
       <c r="B45" s="1"/>
-      <c r="C45" s="16"/>
-      <c r="D45" s="19" t="s">
-        <v>101</v>
-      </c>
-      <c r="E45" s="20" t="n">
+      <c r="C45" s="15"/>
+      <c r="D45" s="18" t="s">
+        <v>99</v>
+      </c>
+      <c r="E45" s="19" t="n">
         <f aca="false">SUM(E7:E22)+SUM(E25:E27)+SUM(E30:E33)+SUM(E36:E41)</f>
         <v>100</v>
       </c>

</xml_diff>